<commit_message>
navbar + un peu de style
</commit_message>
<xml_diff>
--- a/doc/OverwatchCollection_planning.xlsx
+++ b/doc/OverwatchCollection_planning.xlsx
@@ -177,12 +177,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -198,6 +192,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,7 +512,7 @@
   <dimension ref="A1:AO11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -522,182 +522,184 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="s">
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2" t="s">
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2" t="s">
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2" t="s">
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2" t="s">
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="13"/>
+      <c r="AD1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="AE1" s="2"/>
-      <c r="AF1" s="2"/>
-      <c r="AG1" s="2"/>
-      <c r="AH1" s="2" t="s">
+      <c r="AE1" s="13"/>
+      <c r="AF1" s="13"/>
+      <c r="AG1" s="13"/>
+      <c r="AH1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="AI1" s="2"/>
-      <c r="AJ1" s="2"/>
-      <c r="AK1" s="2"/>
-      <c r="AL1" s="2" t="s">
+      <c r="AI1" s="13"/>
+      <c r="AJ1" s="13"/>
+      <c r="AK1" s="13"/>
+      <c r="AL1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="AM1" s="2"/>
-      <c r="AN1" s="2"/>
-      <c r="AO1" s="2"/>
+      <c r="AM1" s="13"/>
+      <c r="AN1" s="13"/>
+      <c r="AO1" s="13"/>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="B2" s="3">
+      <c r="B2" s="14">
         <v>42892</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14">
         <v>42893</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3">
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14">
         <v>42894</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3">
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14">
         <v>42895</v>
       </c>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3">
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14">
         <v>42898</v>
       </c>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3">
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14">
         <v>42899</v>
       </c>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3">
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14">
         <v>42900</v>
       </c>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3">
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
+      <c r="AD2" s="14">
         <v>42901</v>
       </c>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-      <c r="AG2" s="3"/>
-      <c r="AH2" s="3">
+      <c r="AE2" s="14"/>
+      <c r="AF2" s="14"/>
+      <c r="AG2" s="14"/>
+      <c r="AH2" s="14">
         <v>42902</v>
       </c>
-      <c r="AI2" s="3"/>
-      <c r="AJ2" s="3"/>
-      <c r="AK2" s="3"/>
-      <c r="AL2" s="3">
+      <c r="AI2" s="14"/>
+      <c r="AJ2" s="14"/>
+      <c r="AK2" s="14"/>
+      <c r="AL2" s="14">
         <v>42905</v>
       </c>
-      <c r="AM2" s="3"/>
-      <c r="AN2" s="3"/>
-      <c r="AO2" s="3"/>
+      <c r="AM2" s="14"/>
+      <c r="AN2" s="14"/>
+      <c r="AO2" s="14"/>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:41" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:41" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="10"/>
+      <c r="B5" s="8"/>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="11"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:41" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="14"/>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:41" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -706,18 +708,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AL1:AO1"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="Z1:AC1"/>
@@ -726,6 +716,18 @@
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH1:AK1"/>
     <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
index + debut heroes
</commit_message>
<xml_diff>
--- a/doc/OverwatchCollection_planning.xlsx
+++ b/doc/OverwatchCollection_planning.xlsx
@@ -172,32 +172,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO11"/>
+  <dimension ref="A1:AS16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="AL27" sqref="Y15:AL27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -521,193 +518,830 @@
     <col min="2" max="41" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="B1" s="13" t="s">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13" t="s">
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13" t="s">
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13" t="s">
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13" t="s">
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13" t="s">
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="13"/>
-      <c r="AD1" s="13" t="s">
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13" t="s">
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="13"/>
-      <c r="AK1" s="13"/>
-      <c r="AL1" s="13" t="s">
+      <c r="AI1" s="11"/>
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="11"/>
+      <c r="AL1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="AM1" s="13"/>
-      <c r="AN1" s="13"/>
-      <c r="AO1" s="13"/>
-    </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="B2" s="14">
+      <c r="AM1" s="11"/>
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="11"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
+    </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="5">
         <v>42892</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5">
         <v>42893</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14">
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5">
         <v>42894</v>
       </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14">
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5">
         <v>42895</v>
       </c>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14">
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5">
         <v>42898</v>
       </c>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14">
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5">
         <v>42899</v>
       </c>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="14">
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5">
         <v>42900</v>
       </c>
-      <c r="AA2" s="14"/>
-      <c r="AB2" s="14"/>
-      <c r="AC2" s="14"/>
-      <c r="AD2" s="14">
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5">
         <v>42901</v>
       </c>
-      <c r="AE2" s="14"/>
-      <c r="AF2" s="14"/>
-      <c r="AG2" s="14"/>
-      <c r="AH2" s="14">
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="5">
         <v>42902</v>
       </c>
-      <c r="AI2" s="14"/>
-      <c r="AJ2" s="14"/>
-      <c r="AK2" s="14"/>
-      <c r="AL2" s="14">
+      <c r="AI2" s="5"/>
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="5">
         <v>42905</v>
       </c>
-      <c r="AM2" s="14"/>
-      <c r="AN2" s="14"/>
-      <c r="AO2" s="14"/>
-    </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="AM2" s="5"/>
+      <c r="AN2" s="5"/>
+      <c r="AO2" s="5"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="2"/>
+      <c r="AS2" s="2"/>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:41" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="2"/>
+      <c r="AS3" s="2"/>
+    </row>
+    <row r="4" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
-    </row>
-    <row r="5" spans="1:41" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="2"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="2"/>
+      <c r="AO4" s="2"/>
+      <c r="AP4" s="2"/>
+      <c r="AQ4" s="2"/>
+      <c r="AR4" s="2"/>
+      <c r="AS4" s="2"/>
+    </row>
+    <row r="5" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="8"/>
-    </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="2"/>
+      <c r="AK5" s="2"/>
+      <c r="AL5" s="2"/>
+      <c r="AM5" s="2"/>
+      <c r="AN5" s="2"/>
+      <c r="AO5" s="2"/>
+      <c r="AP5" s="2"/>
+      <c r="AQ5" s="2"/>
+      <c r="AR5" s="2"/>
+      <c r="AS5" s="2"/>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:41" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="2"/>
+      <c r="AM6" s="2"/>
+      <c r="AN6" s="2"/>
+      <c r="AO6" s="2"/>
+      <c r="AP6" s="2"/>
+      <c r="AQ6" s="2"/>
+      <c r="AR6" s="2"/>
+      <c r="AS6" s="2"/>
+    </row>
+    <row r="7" spans="1:45" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="1:41" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="2"/>
+      <c r="AK7" s="2"/>
+      <c r="AL7" s="2"/>
+      <c r="AM7" s="2"/>
+      <c r="AN7" s="2"/>
+      <c r="AO7" s="2"/>
+      <c r="AP7" s="2"/>
+      <c r="AQ7" s="2"/>
+      <c r="AR7" s="2"/>
+      <c r="AS7" s="2"/>
+    </row>
+    <row r="8" spans="1:45" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="2"/>
+      <c r="AK8" s="2"/>
+      <c r="AL8" s="2"/>
+      <c r="AM8" s="2"/>
+      <c r="AN8" s="2"/>
+      <c r="AO8" s="2"/>
+      <c r="AP8" s="2"/>
+      <c r="AQ8" s="2"/>
+      <c r="AR8" s="2"/>
+      <c r="AS8" s="2"/>
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2"/>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="2"/>
+      <c r="AJ9" s="2"/>
+      <c r="AK9" s="2"/>
+      <c r="AL9" s="2"/>
+      <c r="AM9" s="2"/>
+      <c r="AN9" s="2"/>
+      <c r="AO9" s="2"/>
+      <c r="AP9" s="2"/>
+      <c r="AQ9" s="2"/>
+      <c r="AR9" s="2"/>
+      <c r="AS9" s="2"/>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-    </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="2"/>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="2"/>
+      <c r="AH10" s="2"/>
+      <c r="AI10" s="2"/>
+      <c r="AJ10" s="2"/>
+      <c r="AK10" s="2"/>
+      <c r="AL10" s="2"/>
+      <c r="AM10" s="2"/>
+      <c r="AN10" s="2"/>
+      <c r="AO10" s="2"/>
+      <c r="AP10" s="2"/>
+      <c r="AQ10" s="2"/>
+      <c r="AR10" s="2"/>
+      <c r="AS10" s="2"/>
+    </row>
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2"/>
+      <c r="AE11" s="2"/>
+      <c r="AF11" s="2"/>
+      <c r="AG11" s="2"/>
+      <c r="AH11" s="2"/>
+      <c r="AI11" s="2"/>
+      <c r="AJ11" s="2"/>
+      <c r="AK11" s="2"/>
+      <c r="AL11" s="2"/>
+      <c r="AM11" s="2"/>
+      <c r="AN11" s="2"/>
+      <c r="AO11" s="2"/>
+      <c r="AP11" s="2"/>
+      <c r="AQ11" s="2"/>
+      <c r="AR11" s="2"/>
+      <c r="AS11" s="2"/>
+    </row>
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="2"/>
+      <c r="AF12" s="2"/>
+      <c r="AG12" s="2"/>
+      <c r="AH12" s="2"/>
+      <c r="AI12" s="2"/>
+      <c r="AJ12" s="2"/>
+      <c r="AK12" s="2"/>
+      <c r="AL12" s="2"/>
+      <c r="AM12" s="2"/>
+      <c r="AN12" s="2"/>
+      <c r="AO12" s="2"/>
+      <c r="AP12" s="2"/>
+      <c r="AQ12" s="2"/>
+      <c r="AR12" s="2"/>
+      <c r="AS12" s="2"/>
+    </row>
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="2"/>
+      <c r="AG13" s="2"/>
+      <c r="AH13" s="2"/>
+      <c r="AI13" s="2"/>
+      <c r="AJ13" s="2"/>
+      <c r="AK13" s="2"/>
+      <c r="AL13" s="2"/>
+      <c r="AM13" s="2"/>
+      <c r="AN13" s="2"/>
+      <c r="AO13" s="2"/>
+      <c r="AP13" s="2"/>
+      <c r="AQ13" s="2"/>
+      <c r="AR13" s="2"/>
+      <c r="AS13" s="2"/>
+    </row>
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="2"/>
+      <c r="AE14" s="2"/>
+      <c r="AF14" s="2"/>
+      <c r="AG14" s="2"/>
+      <c r="AH14" s="2"/>
+      <c r="AI14" s="2"/>
+      <c r="AJ14" s="2"/>
+      <c r="AK14" s="2"/>
+      <c r="AL14" s="2"/>
+      <c r="AM14" s="2"/>
+      <c r="AN14" s="2"/>
+      <c r="AO14" s="2"/>
+      <c r="AP14" s="2"/>
+      <c r="AQ14" s="2"/>
+      <c r="AR14" s="2"/>
+      <c r="AS14" s="2"/>
+    </row>
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="2"/>
+      <c r="AF15" s="2"/>
+      <c r="AG15" s="2"/>
+      <c r="AH15" s="2"/>
+      <c r="AI15" s="2"/>
+      <c r="AJ15" s="2"/>
+      <c r="AK15" s="2"/>
+      <c r="AL15" s="2"/>
+      <c r="AM15" s="2"/>
+      <c r="AN15" s="2"/>
+      <c r="AO15" s="2"/>
+      <c r="AP15" s="2"/>
+      <c r="AQ15" s="2"/>
+      <c r="AR15" s="2"/>
+      <c r="AS15" s="2"/>
+    </row>
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="2"/>
+      <c r="AF16" s="2"/>
+      <c r="AG16" s="2"/>
+      <c r="AH16" s="2"/>
+      <c r="AI16" s="2"/>
+      <c r="AJ16" s="2"/>
+      <c r="AK16" s="2"/>
+      <c r="AL16" s="2"/>
+      <c r="AM16" s="2"/>
+      <c r="AN16" s="2"/>
+      <c r="AO16" s="2"/>
+      <c r="AP16" s="2"/>
+      <c r="AQ16" s="2"/>
+      <c r="AR16" s="2"/>
+      <c r="AS16" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AL1:AO1"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="Z1:AC1"/>
@@ -716,18 +1350,6 @@
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH1:AK1"/>
     <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="J2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
heroes.php + 1/2 hero.php
</commit_message>
<xml_diff>
--- a/doc/OverwatchCollection_planning.xlsx
+++ b/doc/OverwatchCollection_planning.xlsx
@@ -63,9 +63,6 @@
     <t>Web/PHP</t>
   </si>
   <si>
-    <t>Base de données</t>
-  </si>
-  <si>
     <t>Documentation technique</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>Planning courrant</t>
+  </si>
+  <si>
+    <t>Base de données/Requêtes</t>
   </si>
 </sst>
 </file>
@@ -182,19 +182,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,7 +509,7 @@
   <dimension ref="A1:AS16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AL27" sqref="Y15:AL27"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -520,66 +520,66 @@
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11" t="s">
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11" t="s">
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11" t="s">
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11" t="s">
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11" t="s">
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="AA1" s="11"/>
-      <c r="AB1" s="11"/>
-      <c r="AC1" s="11"/>
-      <c r="AD1" s="11" t="s">
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="AE1" s="11"/>
-      <c r="AF1" s="11"/>
-      <c r="AG1" s="11"/>
-      <c r="AH1" s="11" t="s">
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="AI1" s="11"/>
-      <c r="AJ1" s="11"/>
-      <c r="AK1" s="11"/>
-      <c r="AL1" s="11" t="s">
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="AM1" s="11"/>
-      <c r="AN1" s="11"/>
-      <c r="AO1" s="11"/>
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="12"/>
       <c r="AP1" s="2"/>
       <c r="AQ1" s="2"/>
       <c r="AR1" s="2"/>
@@ -587,66 +587,66 @@
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="5">
+      <c r="B2" s="13">
         <v>42892</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13">
         <v>42893</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5">
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13">
         <v>42894</v>
       </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5">
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13">
         <v>42895</v>
       </c>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5">
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13">
         <v>42898</v>
       </c>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5">
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13">
         <v>42899</v>
       </c>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5">
+      <c r="W2" s="13"/>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13">
         <v>42900</v>
       </c>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="5"/>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5">
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="13"/>
+      <c r="AC2" s="13"/>
+      <c r="AD2" s="13">
         <v>42901</v>
       </c>
-      <c r="AE2" s="5"/>
-      <c r="AF2" s="5"/>
-      <c r="AG2" s="5"/>
-      <c r="AH2" s="5">
+      <c r="AE2" s="13"/>
+      <c r="AF2" s="13"/>
+      <c r="AG2" s="13"/>
+      <c r="AH2" s="13">
         <v>42902</v>
       </c>
-      <c r="AI2" s="5"/>
-      <c r="AJ2" s="5"/>
-      <c r="AK2" s="5"/>
-      <c r="AL2" s="5">
+      <c r="AI2" s="13"/>
+      <c r="AJ2" s="13"/>
+      <c r="AK2" s="13"/>
+      <c r="AL2" s="13">
         <v>42905</v>
       </c>
-      <c r="AM2" s="5"/>
-      <c r="AN2" s="5"/>
-      <c r="AO2" s="5"/>
+      <c r="AM2" s="13"/>
+      <c r="AN2" s="13"/>
+      <c r="AO2" s="13"/>
       <c r="AP2" s="2"/>
       <c r="AQ2" s="2"/>
       <c r="AR2" s="2"/>
@@ -656,12 +656,12 @@
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -705,12 +705,12 @@
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -752,14 +752,14 @@
     </row>
     <row r="5" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="12"/>
+        <v>18</v>
+      </c>
+      <c r="B5" s="10"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="8"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -850,7 +850,7 @@
     </row>
     <row r="7" spans="1:45" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -899,7 +899,7 @@
     </row>
     <row r="8" spans="1:45" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -950,14 +950,14 @@
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -997,16 +997,16 @@
     </row>
     <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -1330,18 +1330,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AL1:AO1"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="Z1:AC1"/>
@@ -1350,6 +1338,18 @@
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH1:AK1"/>
     <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
my account info + my account update
</commit_message>
<xml_diff>
--- a/doc/OverwatchCollection_planning.xlsx
+++ b/doc/OverwatchCollection_planning.xlsx
@@ -509,7 +509,7 @@
   <dimension ref="A1:AS16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -667,7 +667,7 @@
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
+      <c r="M3" s="5"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
@@ -716,7 +716,7 @@
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
+      <c r="M4" s="6"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
@@ -765,7 +765,7 @@
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
+      <c r="M5" s="10"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
@@ -813,8 +813,8 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
@@ -862,8 +862,8 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
@@ -1330,6 +1330,18 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AL1:AO1"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="Z1:AC1"/>
@@ -1338,18 +1350,6 @@
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH1:AK1"/>
     <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="J2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
admin.php: read, ban, unban
</commit_message>
<xml_diff>
--- a/doc/OverwatchCollection_planning.xlsx
+++ b/doc/OverwatchCollection_planning.xlsx
@@ -509,7 +509,7 @@
   <dimension ref="A1:AS16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -668,8 +668,8 @@
       <c r="K3" s="5"/>
       <c r="L3" s="2"/>
       <c r="M3" s="5"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
@@ -717,8 +717,8 @@
       <c r="K4" s="6"/>
       <c r="L4" s="2"/>
       <c r="M4" s="6"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
@@ -766,8 +766,8 @@
       <c r="K5" s="10"/>
       <c r="L5" s="2"/>
       <c r="M5" s="10"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
@@ -962,8 +962,8 @@
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
@@ -1011,8 +1011,8 @@
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
@@ -1330,18 +1330,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AL1:AO1"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="Z1:AC1"/>
@@ -1350,6 +1338,18 @@
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH1:AK1"/>
     <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
maquettes index ... -> events
</commit_message>
<xml_diff>
--- a/doc/OverwatchCollection_planning.xlsx
+++ b/doc/OverwatchCollection_planning.xlsx
@@ -509,7 +509,7 @@
   <dimension ref="A1:AS16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -817,7 +817,7 @@
       <c r="M6" s="7"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
+      <c r="P6" s="7"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
@@ -866,7 +866,7 @@
       <c r="M7" s="4"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
+      <c r="P7" s="4"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
@@ -1330,6 +1330,18 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AL1:AO1"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="Z1:AC1"/>
@@ -1338,18 +1350,6 @@
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH1:AK1"/>
     <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="J2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fonction add_user_reward -> hero et event
</commit_message>
<xml_diff>
--- a/doc/OverwatchCollection_planning.xlsx
+++ b/doc/OverwatchCollection_planning.xlsx
@@ -509,7 +509,7 @@
   <dimension ref="A1:AS16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -671,7 +671,7 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
+      <c r="Q3" s="5"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
@@ -720,7 +720,7 @@
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
       <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
+      <c r="Q4" s="6"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
@@ -769,7 +769,7 @@
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
       <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
+      <c r="Q5" s="10"/>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
@@ -818,7 +818,7 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="7"/>
-      <c r="Q6" s="2"/>
+      <c r="Q6" s="7"/>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
@@ -867,7 +867,7 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="4"/>
-      <c r="Q7" s="2"/>
+      <c r="Q7" s="4"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
@@ -964,8 +964,8 @@
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
@@ -1013,8 +1013,8 @@
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
@@ -1330,18 +1330,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AL1:AO1"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="Z1:AC1"/>
@@ -1350,6 +1338,18 @@
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH1:AK1"/>
     <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fonction display + lien rewards que quandconecté
</commit_message>
<xml_diff>
--- a/doc/OverwatchCollection_planning.xlsx
+++ b/doc/OverwatchCollection_planning.xlsx
@@ -509,7 +509,7 @@
   <dimension ref="A1:AS16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -672,7 +672,7 @@
       <c r="O3" s="5"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="5"/>
-      <c r="R3" s="2"/>
+      <c r="R3" s="5"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
@@ -721,7 +721,7 @@
       <c r="O4" s="6"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="6"/>
-      <c r="R4" s="2"/>
+      <c r="R4" s="6"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
@@ -770,7 +770,7 @@
       <c r="O5" s="10"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="10"/>
-      <c r="R5" s="2"/>
+      <c r="R5" s="10"/>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
@@ -966,7 +966,7 @@
       <c r="O9" s="8"/>
       <c r="P9" s="8"/>
       <c r="Q9" s="8"/>
-      <c r="R9" s="2"/>
+      <c r="R9" s="11"/>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
@@ -1015,7 +1015,7 @@
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
-      <c r="R10" s="2"/>
+      <c r="R10" s="9"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
@@ -1330,6 +1330,18 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AL1:AO1"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="Z1:AC1"/>
@@ -1338,18 +1350,6 @@
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH1:AK1"/>
     <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="J2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
maquette preli + doc
</commit_message>
<xml_diff>
--- a/doc/OverwatchCollection_planning.xlsx
+++ b/doc/OverwatchCollection_planning.xlsx
@@ -509,7 +509,7 @@
   <dimension ref="A1:AS16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+      <selection activeCell="AB8" sqref="AB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -820,7 +820,7 @@
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
+      <c r="S6" s="7"/>
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
@@ -869,7 +869,7 @@
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
+      <c r="S7" s="4"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
@@ -967,7 +967,7 @@
       <c r="P9" s="8"/>
       <c r="Q9" s="8"/>
       <c r="R9" s="11"/>
-      <c r="S9" s="2"/>
+      <c r="S9" s="8"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
@@ -1016,7 +1016,7 @@
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
       <c r="R10" s="9"/>
-      <c r="S10" s="2"/>
+      <c r="S10" s="9"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
@@ -1330,18 +1330,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AL1:AO1"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="Z1:AC1"/>
@@ -1350,6 +1338,18 @@
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH1:AK1"/>
     <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
progress bar main + event
</commit_message>
<xml_diff>
--- a/doc/OverwatchCollection_planning.xlsx
+++ b/doc/OverwatchCollection_planning.xlsx
@@ -509,7 +509,7 @@
   <dimension ref="A1:AS16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB8" sqref="AB8"/>
+      <selection activeCell="V3" sqref="V3:V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -675,8 +675,8 @@
       <c r="R3" s="5"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
@@ -724,8 +724,8 @@
       <c r="R4" s="6"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
@@ -773,8 +773,8 @@
       <c r="R5" s="10"/>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
@@ -821,7 +821,7 @@
       <c r="Q6" s="7"/>
       <c r="R6" s="2"/>
       <c r="S6" s="7"/>
-      <c r="T6" s="2"/>
+      <c r="T6" s="7"/>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
@@ -870,7 +870,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="2"/>
       <c r="S7" s="4"/>
-      <c r="T7" s="2"/>
+      <c r="T7" s="4"/>
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
@@ -968,9 +968,9 @@
       <c r="Q9" s="8"/>
       <c r="R9" s="11"/>
       <c r="S9" s="8"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
@@ -1017,9 +1017,9 @@
       <c r="Q10" s="9"/>
       <c r="R10" s="9"/>
       <c r="S10" s="9"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
@@ -1330,6 +1330,18 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AL1:AO1"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="Z1:AC1"/>
@@ -1338,18 +1350,6 @@
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH1:AK1"/>
     <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="J2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
doc explication requête sql fin
</commit_message>
<xml_diff>
--- a/doc/OverwatchCollection_planning.xlsx
+++ b/doc/OverwatchCollection_planning.xlsx
@@ -509,7 +509,7 @@
   <dimension ref="A1:AS16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3:V10"/>
+      <selection activeCell="Y3" sqref="Y3:Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -679,7 +679,7 @@
       <c r="V3" s="5"/>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
+      <c r="Y3" s="5"/>
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
@@ -728,7 +728,7 @@
       <c r="V4" s="6"/>
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
+      <c r="Y4" s="6"/>
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
@@ -777,7 +777,7 @@
       <c r="V5" s="10"/>
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
+      <c r="Y5" s="10"/>
       <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
@@ -824,9 +824,9 @@
       <c r="T6" s="7"/>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
@@ -873,9 +873,9 @@
       <c r="T7" s="4"/>
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
@@ -971,9 +971,9 @@
       <c r="T9" s="8"/>
       <c r="U9" s="11"/>
       <c r="V9" s="11"/>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="2"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8"/>
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
@@ -1020,9 +1020,9 @@
       <c r="T10" s="9"/>
       <c r="U10" s="9"/>
       <c r="V10" s="9"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="2"/>
-      <c r="Y10" s="2"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
@@ -1330,18 +1330,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AL1:AO1"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="Z1:AC1"/>
@@ -1350,6 +1338,18 @@
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH1:AK1"/>
     <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
class display + rangement code
</commit_message>
<xml_diff>
--- a/doc/OverwatchCollection_planning.xlsx
+++ b/doc/OverwatchCollection_planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve"> Jour 1</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Base de données/Requêtes</t>
+  </si>
+  <si>
+    <t>Rangement de code</t>
   </si>
 </sst>
 </file>
@@ -110,7 +113,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,6 +162,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA469D1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -172,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -195,6 +204,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -203,6 +215,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FFA469D1"/>
+      <color rgb="FF9E5ECE"/>
       <color rgb="FF0594FF"/>
       <color rgb="FF0083E6"/>
       <color rgb="FFFF5001"/>
@@ -506,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS16"/>
+  <dimension ref="A1:AS17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3:Y10"/>
+      <selection activeCell="AI7" sqref="AI7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -680,8 +694,8 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="5"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
@@ -729,7 +743,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="6"/>
-      <c r="Z4" s="2"/>
+      <c r="Z4" s="14"/>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
@@ -778,7 +792,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
       <c r="Y5" s="10"/>
-      <c r="Z5" s="2"/>
+      <c r="Z5" s="14"/>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
@@ -799,36 +813,36 @@
       <c r="AR5" s="2"/>
       <c r="AS5" s="2"/>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="2"/>
-      <c r="AA6" s="2"/>
+    <row r="6" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="16"/>
+      <c r="AA6" s="16"/>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
@@ -848,36 +862,36 @@
       <c r="AR6" s="2"/>
       <c r="AS6" s="2"/>
     </row>
-    <row r="7" spans="1:45" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="4"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="7"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
       <c r="R7" s="2"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
-      <c r="W7" s="4"/>
-      <c r="X7" s="4"/>
-      <c r="Y7" s="4"/>
-      <c r="Z7" s="2"/>
-      <c r="AA7" s="2"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="7"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
       <c r="AD7" s="2"/>
@@ -899,34 +913,34 @@
     </row>
     <row r="8" spans="1:45" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="D8" s="4"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="H8" s="4"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
       <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2"/>
-      <c r="AA8" s="2"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="4"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
       <c r="AD8" s="2"/>
@@ -946,34 +960,34 @@
       <c r="AR8" s="2"/>
       <c r="AS8" s="2"/>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="8"/>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="8"/>
+    <row r="9" spans="1:45" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
@@ -996,35 +1010,35 @@
       <c r="AS9" s="2"/>
     </row>
     <row r="10" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="9"/>
-      <c r="X10" s="9"/>
-      <c r="Y10" s="9"/>
-      <c r="Z10" s="2"/>
-      <c r="AA10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
       <c r="AD10" s="2"/>
@@ -1045,35 +1059,35 @@
       <c r="AS10" s="2"/>
     </row>
     <row r="11" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-      <c r="X11" s="2"/>
-      <c r="Y11" s="2"/>
-      <c r="Z11" s="2"/>
-      <c r="AA11" s="2"/>
+      <c r="A11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
       <c r="AD11" s="2"/>
@@ -1094,7 +1108,9 @@
       <c r="AS11" s="2"/>
     </row>
     <row r="12" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1328,8 +1344,67 @@
       <c r="AR16" s="2"/>
       <c r="AS16" s="2"/>
     </row>
+    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="2"/>
+      <c r="AE17" s="2"/>
+      <c r="AF17" s="2"/>
+      <c r="AG17" s="2"/>
+      <c r="AH17" s="2"/>
+      <c r="AI17" s="2"/>
+      <c r="AJ17" s="2"/>
+      <c r="AK17" s="2"/>
+      <c r="AL17" s="2"/>
+      <c r="AM17" s="2"/>
+      <c r="AN17" s="2"/>
+      <c r="AO17" s="2"/>
+      <c r="AP17" s="2"/>
+      <c r="AQ17" s="2"/>
+      <c r="AR17" s="2"/>
+      <c r="AS17" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AL1:AO1"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="Z1:AC1"/>
@@ -1338,18 +1413,6 @@
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH1:AK1"/>
     <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="J2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>